<commit_message>
Removed time tags from concordances for easier adaptations. There seems to be a problem with the long rolled product data feed, specifically regarding the zero's.
</commit_message>
<xml_diff>
--- a/ConcordanceLibrary/Additional/20200426_Additional_Root2Mother_Sec_Ind30Pro39v1.xlsx
+++ b/ConcordanceLibrary/Additional/20200426_Additional_Root2Mother_Sec_Ind30Pro39v1.xlsx
@@ -5303,10 +5303,10 @@
   <dimension ref="A1:T268"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C228" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C151" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="R249" sqref="R249"/>
+      <selection pane="bottomRight" activeCell="F153" sqref="F153"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>